<commit_message>
improved formatting of excel files
</commit_message>
<xml_diff>
--- a/estimates/G8.xlsx
+++ b/estimates/G8.xlsx
@@ -550,8 +550,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -875,9 +878,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="33.140625" customWidth="1"/>
+    <col min="13" max="13" width="58.7109375" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -910,13 +930,13 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -933,7 +953,7 @@
       <c r="J2">
         <v>1</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="L2" t="s">

</xml_diff>